<commit_message>
multiple changes. Enriching data, improving visualizations, creating requirements.txt, and others
</commit_message>
<xml_diff>
--- a/data/results/nearest_neighbors.xlsx
+++ b/data/results/nearest_neighbors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrac\Documents\Uni\Masterarbeit\migration_im_Bundestag\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584C18BC-5519-41D2-B9F0-7CA411671012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9685B6D-D8CD-4B32-AD2B-9FEDF56C0CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,11 @@
     <sheet name="explanations" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="1016">
   <si>
     <t>Keyword</t>
   </si>
@@ -3046,6 +3045,30 @@
   </si>
   <si>
     <t>Frau Ursula Kugler, Abgeordnete.</t>
+  </si>
+  <si>
+    <t>palästinensisches Flüchtlingslager Jarmuk in Syrien</t>
+  </si>
+  <si>
+    <t>Syrien-Krieg, IS</t>
+  </si>
+  <si>
+    <t>Tippfehler: "daß Sie sich dahintersteliten". --&gt; "dahinterstellten" gemeint. Bildungspolitische Diskussion</t>
+  </si>
+  <si>
+    <t>Mario Soares, ehemaliger portugiesischer Politiker. Europapolitik</t>
+  </si>
+  <si>
+    <t>"Leher Bahnhof", Gelände in Bremen</t>
+  </si>
+  <si>
+    <t>Gelände soll für Wohnungen für "Altbesatzungsverdrängte" umgebaut werden</t>
+  </si>
+  <si>
+    <t>Jever, Stadt/Region</t>
+  </si>
+  <si>
+    <t>von Motz, wahrscheinlich Friedrich von Motz, Eisenbahn</t>
   </si>
 </sst>
 </file>
@@ -3209,7 +3232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3401,6 +3424,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3574,7 +3603,7 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3933,8 +3962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V133"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5993,13 +6022,13 @@
       <c r="B31" s="3">
         <v>8</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="6" t="s">
         <v>146</v>
       </c>
       <c r="D31" s="3">
         <v>0.73560452461242598</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="6" t="s">
         <v>147</v>
       </c>
       <c r="F31" s="3">
@@ -6061,13 +6090,13 @@
       <c r="B32" s="3">
         <v>1</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="6" t="s">
         <v>153</v>
       </c>
       <c r="D32" s="3">
         <v>0.60769408941268899</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="6" t="s">
         <v>154</v>
       </c>
       <c r="F32" s="3">
@@ -6339,7 +6368,7 @@
       <c r="D36" s="3">
         <v>0.59148430824279696</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="3" t="s">
         <v>188</v>
       </c>
       <c r="F36" s="3">
@@ -12997,10 +13026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13239,7 +13268,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="3" t="s">
         <v>778</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -13802,6 +13831,156 @@
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="C33" s="9">
+        <v>7</v>
+      </c>
+      <c r="D33" s="9">
+        <v>2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>6</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="9">
+        <v>8</v>
+      </c>
+      <c r="D34" s="9">
+        <v>3</v>
+      </c>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="9">
+        <v>2</v>
+      </c>
+      <c r="D35" s="9">
+        <v>3</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="3">
+        <v>6</v>
+      </c>
+      <c r="D36" s="3">
+        <v>3</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>1015</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>